<commit_message>
Add tests, documents, timers
</commit_message>
<xml_diff>
--- a/PBNA*/Documentation/tests/Tests.xlsx
+++ b/PBNA*/Documentation/tests/Tests.xlsx
@@ -5,16 +5,31 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alejandrogleason/Desktop/ITESM/7moSemestre/Languages/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alejandrogleason/Desktop/ITESM/7moSemestre/Languages/MAPFAstar/PBNA*/Documentation/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC6940AB-CE22-0448-BB87-D4F09A3B0204}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5D37FF2-01F8-1545-B8B9-0C7A61746469}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="500" windowWidth="19180" windowHeight="21100" xr2:uid="{30FD93A9-A9E8-2C49-96BE-D163A867F6E4}"/>
+    <workbookView xWindow="-22540" yWindow="500" windowWidth="23360" windowHeight="21100" xr2:uid="{30FD93A9-A9E8-2C49-96BE-D163A867F6E4}"/>
   </bookViews>
   <sheets>
-    <sheet name="15x15 grid" sheetId="1" r:id="rId1"/>
+    <sheet name="Tests" sheetId="1" r:id="rId1"/>
+    <sheet name="Graphs" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.10" hidden="1">Graphs!$D$26</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Graphs!$D$27:$D$33</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Graphs!$B$26</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Graphs!$B$27:$B$33</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Graphs!$C$26</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Graphs!$C$27:$C$33</definedName>
+    <definedName name="_xlchart.v2.0" hidden="1">Graphs!$B$26</definedName>
+    <definedName name="_xlchart.v2.1" hidden="1">Graphs!$B$27:$B$33</definedName>
+    <definedName name="_xlchart.v2.2" hidden="1">Graphs!$C$26</definedName>
+    <definedName name="_xlchart.v2.3" hidden="1">Graphs!$C$27:$C$33</definedName>
+    <definedName name="_xlchart.v2.4" hidden="1">Graphs!$D$26</definedName>
+    <definedName name="_xlchart.v2.5" hidden="1">Graphs!$D$27:$D$33</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="30">
   <si>
     <t>init</t>
   </si>
@@ -98,12 +113,39 @@
   <si>
     <t>4, 2</t>
   </si>
+  <si>
+    <t>0, 0</t>
+  </si>
+  <si>
+    <t>3, 13</t>
+  </si>
+  <si>
+    <t>9, 12</t>
+  </si>
+  <si>
+    <t>Size of grid</t>
+  </si>
+  <si>
+    <t>Success rate</t>
+  </si>
+  <si>
+    <t>Avg. execution time seq</t>
+  </si>
+  <si>
+    <t>time (s)</t>
+  </si>
+  <si>
+    <t>grid size</t>
+  </si>
+  <si>
+    <t>Avg. execution time multithreaded</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -125,8 +167,14 @@
       <name val="Menlo"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Century Gothic"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -148,6 +196,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -210,7 +264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -226,6 +280,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -241,6 +304,2060 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Graphs!$C$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Success rate</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="15875" cap="rnd">
+                <a:noFill/>
+                <a:prstDash val="dash"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Graphs!$B$5:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>255</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>288</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>324</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Graphs!$C$5:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.69</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A398-1340-8CD6-7BC60D822408}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1501495488"/>
+        <c:axId val="1501091504"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1501495488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1501091504"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1501091504"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1501495488"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:srgbClr val="FF0000"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-MX"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="70" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Running</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Times</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="70" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Graphs!$C$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Avg. execution time seq</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:alpha val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Graphs!$B$27:$B$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>255</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>288</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>324</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Graphs!$C$27:$C$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>3.256E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.512E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5699999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.8699999999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.5E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.1419999999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.8749999999999996E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7928-7442-9BEA-568665A92E42}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Graphs!$D$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Avg. execution time multithreaded</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:alpha val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Graphs!$B$27:$B$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>255</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>288</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>324</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Graphs!$D$27:$D$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>6.5199999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.304E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.9999999999999997E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.8999999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.5419999999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.3849999999999996E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7928-7442-9BEA-568665A92E42}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1526192432"/>
+        <c:axId val="1525739600"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1526192432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1525739600"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1525739600"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1526192432"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="100000">
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="43000">
+          <a:schemeClr val="lt1"/>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-MX"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="241">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="244">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="95000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="43000">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="20000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="0" kern="1200" spc="70" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="63500" cap="rnd" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>289214</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>733714</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50D0F73D-BFE6-A149-B022-276FEB5D9D83}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>465666</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>37907</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>105830</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{104B9B32-D5FB-4E44-8DF0-90A804682014}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -540,10 +2657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAA5A4F6-75D1-3747-B9DA-4AC478A23F48}">
-  <dimension ref="A1:R160"/>
+  <dimension ref="A1:R183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A135" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="65" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="M101" sqref="M101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6558,7 +8675,1412 @@
         <v>1</v>
       </c>
     </row>
+    <row r="163" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B163" s="1">
+        <v>0</v>
+      </c>
+      <c r="C163" s="1">
+        <v>1</v>
+      </c>
+      <c r="D163" s="1">
+        <v>2</v>
+      </c>
+      <c r="E163" s="1">
+        <v>3</v>
+      </c>
+      <c r="F163" s="1">
+        <v>4</v>
+      </c>
+      <c r="G163" s="1">
+        <v>5</v>
+      </c>
+      <c r="H163" s="1">
+        <v>6</v>
+      </c>
+      <c r="I163" s="1">
+        <v>7</v>
+      </c>
+      <c r="J163" s="1">
+        <v>8</v>
+      </c>
+      <c r="K163" s="1">
+        <v>9</v>
+      </c>
+      <c r="L163" s="1">
+        <v>10</v>
+      </c>
+      <c r="M163" s="1">
+        <v>11</v>
+      </c>
+      <c r="N163" s="1">
+        <v>12</v>
+      </c>
+      <c r="O163" s="1">
+        <v>13</v>
+      </c>
+      <c r="P163" s="1">
+        <v>14</v>
+      </c>
+      <c r="Q163" s="1"/>
+    </row>
+    <row r="164" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A164" s="1">
+        <v>0</v>
+      </c>
+      <c r="B164" s="13">
+        <v>0</v>
+      </c>
+      <c r="C164" s="4">
+        <v>0</v>
+      </c>
+      <c r="D164" s="4">
+        <v>0</v>
+      </c>
+      <c r="E164" s="4">
+        <v>0</v>
+      </c>
+      <c r="F164" s="4">
+        <v>0</v>
+      </c>
+      <c r="G164" s="4">
+        <v>0</v>
+      </c>
+      <c r="H164" s="4">
+        <v>0</v>
+      </c>
+      <c r="I164" s="5">
+        <v>1</v>
+      </c>
+      <c r="J164" s="5">
+        <v>0</v>
+      </c>
+      <c r="K164" s="5">
+        <v>1</v>
+      </c>
+      <c r="L164" s="5">
+        <v>1</v>
+      </c>
+      <c r="M164" s="5">
+        <v>0</v>
+      </c>
+      <c r="N164" s="5">
+        <v>1</v>
+      </c>
+      <c r="O164" s="5">
+        <v>0</v>
+      </c>
+      <c r="P164" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A165" s="1">
+        <v>1</v>
+      </c>
+      <c r="B165" s="15">
+        <v>0</v>
+      </c>
+      <c r="C165" s="15">
+        <v>0</v>
+      </c>
+      <c r="D165" s="15">
+        <v>1</v>
+      </c>
+      <c r="E165" s="15">
+        <v>0</v>
+      </c>
+      <c r="F165" s="15">
+        <v>1</v>
+      </c>
+      <c r="G165" s="15">
+        <v>0</v>
+      </c>
+      <c r="H165" s="16">
+        <v>0</v>
+      </c>
+      <c r="I165" s="16">
+        <v>0</v>
+      </c>
+      <c r="J165" s="16">
+        <v>0</v>
+      </c>
+      <c r="K165" s="15">
+        <v>0</v>
+      </c>
+      <c r="L165" s="15">
+        <v>1</v>
+      </c>
+      <c r="M165" s="15">
+        <v>1</v>
+      </c>
+      <c r="N165" s="15">
+        <v>1</v>
+      </c>
+      <c r="O165" s="15">
+        <v>0</v>
+      </c>
+      <c r="P165" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A166" s="1">
+        <v>2</v>
+      </c>
+      <c r="B166" s="15">
+        <v>0</v>
+      </c>
+      <c r="C166" s="15">
+        <v>0</v>
+      </c>
+      <c r="D166" s="15">
+        <v>0</v>
+      </c>
+      <c r="E166" s="15">
+        <v>0</v>
+      </c>
+      <c r="F166" s="15">
+        <v>0</v>
+      </c>
+      <c r="G166" s="15">
+        <v>0</v>
+      </c>
+      <c r="H166" s="15">
+        <v>0</v>
+      </c>
+      <c r="I166" s="15">
+        <v>1</v>
+      </c>
+      <c r="J166" s="16">
+        <v>0</v>
+      </c>
+      <c r="K166" s="15">
+        <v>0</v>
+      </c>
+      <c r="L166" s="15">
+        <v>1</v>
+      </c>
+      <c r="M166" s="15">
+        <v>1</v>
+      </c>
+      <c r="N166" s="15">
+        <v>0</v>
+      </c>
+      <c r="O166" s="15">
+        <v>0</v>
+      </c>
+      <c r="P166" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A167" s="1">
+        <v>3</v>
+      </c>
+      <c r="B167" s="15">
+        <v>0</v>
+      </c>
+      <c r="C167" s="15">
+        <v>1</v>
+      </c>
+      <c r="D167" s="15">
+        <v>0</v>
+      </c>
+      <c r="E167" s="15">
+        <v>0</v>
+      </c>
+      <c r="F167" s="15">
+        <v>1</v>
+      </c>
+      <c r="G167" s="15">
+        <v>0</v>
+      </c>
+      <c r="H167" s="15">
+        <v>0</v>
+      </c>
+      <c r="I167" s="15">
+        <v>1</v>
+      </c>
+      <c r="J167" s="16">
+        <v>0</v>
+      </c>
+      <c r="K167" s="15">
+        <v>1</v>
+      </c>
+      <c r="L167" s="15">
+        <v>0</v>
+      </c>
+      <c r="M167" s="16">
+        <v>0</v>
+      </c>
+      <c r="N167" s="16">
+        <v>0</v>
+      </c>
+      <c r="O167" s="13">
+        <v>0</v>
+      </c>
+      <c r="P167" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A168" s="1">
+        <v>4</v>
+      </c>
+      <c r="B168" s="15">
+        <v>0</v>
+      </c>
+      <c r="C168" s="15">
+        <v>0</v>
+      </c>
+      <c r="D168" s="15">
+        <v>0</v>
+      </c>
+      <c r="E168" s="15">
+        <v>0</v>
+      </c>
+      <c r="F168" s="15">
+        <v>0</v>
+      </c>
+      <c r="G168" s="15">
+        <v>0</v>
+      </c>
+      <c r="H168" s="15">
+        <v>1</v>
+      </c>
+      <c r="I168" s="15">
+        <v>0</v>
+      </c>
+      <c r="J168" s="16">
+        <v>0</v>
+      </c>
+      <c r="K168" s="16">
+        <v>0</v>
+      </c>
+      <c r="L168" s="16">
+        <v>0</v>
+      </c>
+      <c r="M168" s="16">
+        <v>0</v>
+      </c>
+      <c r="N168" s="15">
+        <v>0</v>
+      </c>
+      <c r="O168" s="15">
+        <v>1</v>
+      </c>
+      <c r="P168" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A169" s="1">
+        <v>5</v>
+      </c>
+      <c r="B169" s="15">
+        <v>0</v>
+      </c>
+      <c r="C169" s="15">
+        <v>1</v>
+      </c>
+      <c r="D169" s="15">
+        <v>0</v>
+      </c>
+      <c r="E169" s="15">
+        <v>0</v>
+      </c>
+      <c r="F169" s="15">
+        <v>1</v>
+      </c>
+      <c r="G169" s="15">
+        <v>0</v>
+      </c>
+      <c r="H169" s="15">
+        <v>0</v>
+      </c>
+      <c r="I169" s="15">
+        <v>0</v>
+      </c>
+      <c r="J169" s="15">
+        <v>1</v>
+      </c>
+      <c r="K169" s="15">
+        <v>1</v>
+      </c>
+      <c r="L169" s="15">
+        <v>1</v>
+      </c>
+      <c r="M169" s="15">
+        <v>0</v>
+      </c>
+      <c r="N169" s="15">
+        <v>1</v>
+      </c>
+      <c r="O169" s="15">
+        <v>0</v>
+      </c>
+      <c r="P169" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A170" s="1">
+        <v>6</v>
+      </c>
+      <c r="B170" s="15">
+        <v>0</v>
+      </c>
+      <c r="C170" s="15">
+        <v>0</v>
+      </c>
+      <c r="D170" s="15">
+        <v>0</v>
+      </c>
+      <c r="E170" s="15">
+        <v>0</v>
+      </c>
+      <c r="F170" s="15">
+        <v>0</v>
+      </c>
+      <c r="G170" s="15">
+        <v>0</v>
+      </c>
+      <c r="H170" s="15">
+        <v>0</v>
+      </c>
+      <c r="I170" s="15">
+        <v>1</v>
+      </c>
+      <c r="J170" s="15">
+        <v>1</v>
+      </c>
+      <c r="K170" s="15">
+        <v>0</v>
+      </c>
+      <c r="L170" s="15">
+        <v>1</v>
+      </c>
+      <c r="M170" s="15">
+        <v>1</v>
+      </c>
+      <c r="N170" s="15">
+        <v>0</v>
+      </c>
+      <c r="O170" s="15">
+        <v>0</v>
+      </c>
+      <c r="P170" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A171" s="1">
+        <v>7</v>
+      </c>
+      <c r="B171" s="15">
+        <v>1</v>
+      </c>
+      <c r="C171" s="15">
+        <v>0</v>
+      </c>
+      <c r="D171" s="15">
+        <v>1</v>
+      </c>
+      <c r="E171" s="15">
+        <v>0</v>
+      </c>
+      <c r="F171" s="15">
+        <v>1</v>
+      </c>
+      <c r="G171" s="15">
+        <v>0</v>
+      </c>
+      <c r="H171" s="15">
+        <v>0</v>
+      </c>
+      <c r="I171" s="15">
+        <v>0</v>
+      </c>
+      <c r="J171" s="15">
+        <v>0</v>
+      </c>
+      <c r="K171" s="15">
+        <v>1</v>
+      </c>
+      <c r="L171" s="15">
+        <v>0</v>
+      </c>
+      <c r="M171" s="15">
+        <v>0</v>
+      </c>
+      <c r="N171" s="15">
+        <v>0</v>
+      </c>
+      <c r="O171" s="15">
+        <v>0</v>
+      </c>
+      <c r="P171" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A172" s="1">
+        <v>8</v>
+      </c>
+      <c r="B172" s="15">
+        <v>0</v>
+      </c>
+      <c r="C172" s="15">
+        <v>1</v>
+      </c>
+      <c r="D172" s="15">
+        <v>0</v>
+      </c>
+      <c r="E172" s="15">
+        <v>0</v>
+      </c>
+      <c r="F172" s="15">
+        <v>1</v>
+      </c>
+      <c r="G172" s="15">
+        <v>0</v>
+      </c>
+      <c r="H172" s="15">
+        <v>0</v>
+      </c>
+      <c r="I172" s="15">
+        <v>1</v>
+      </c>
+      <c r="J172" s="15">
+        <v>0</v>
+      </c>
+      <c r="K172" s="15">
+        <v>1</v>
+      </c>
+      <c r="L172" s="15">
+        <v>0</v>
+      </c>
+      <c r="M172" s="15">
+        <v>0</v>
+      </c>
+      <c r="N172" s="15">
+        <v>1</v>
+      </c>
+      <c r="O172" s="15">
+        <v>0</v>
+      </c>
+      <c r="P172" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A173" s="1">
+        <v>9</v>
+      </c>
+      <c r="B173" s="15">
+        <v>0</v>
+      </c>
+      <c r="C173" s="15">
+        <v>0</v>
+      </c>
+      <c r="D173" s="15">
+        <v>0</v>
+      </c>
+      <c r="E173" s="15">
+        <v>0</v>
+      </c>
+      <c r="F173" s="15">
+        <v>0</v>
+      </c>
+      <c r="G173" s="15">
+        <v>0</v>
+      </c>
+      <c r="H173" s="15">
+        <v>1</v>
+      </c>
+      <c r="I173" s="15">
+        <v>0</v>
+      </c>
+      <c r="J173" s="15">
+        <v>0</v>
+      </c>
+      <c r="K173" s="15">
+        <v>0</v>
+      </c>
+      <c r="L173" s="17">
+        <v>0</v>
+      </c>
+      <c r="M173" s="17">
+        <v>0</v>
+      </c>
+      <c r="N173" s="12">
+        <v>0</v>
+      </c>
+      <c r="O173" s="15">
+        <v>1</v>
+      </c>
+      <c r="P173" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A174" s="1">
+        <v>10</v>
+      </c>
+      <c r="B174" s="15">
+        <v>0</v>
+      </c>
+      <c r="C174" s="15">
+        <v>0</v>
+      </c>
+      <c r="D174" s="15">
+        <v>1</v>
+      </c>
+      <c r="E174" s="15">
+        <v>0</v>
+      </c>
+      <c r="F174" s="15">
+        <v>1</v>
+      </c>
+      <c r="G174" s="15">
+        <v>0</v>
+      </c>
+      <c r="H174" s="15">
+        <v>0</v>
+      </c>
+      <c r="I174" s="15">
+        <v>0</v>
+      </c>
+      <c r="J174" s="17">
+        <v>0</v>
+      </c>
+      <c r="K174" s="17">
+        <v>0</v>
+      </c>
+      <c r="L174" s="17">
+        <v>0</v>
+      </c>
+      <c r="M174" s="15">
+        <v>1</v>
+      </c>
+      <c r="N174" s="15">
+        <v>0</v>
+      </c>
+      <c r="O174" s="15">
+        <v>1</v>
+      </c>
+      <c r="P174" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A175" s="1">
+        <v>11</v>
+      </c>
+      <c r="B175" s="15">
+        <v>0</v>
+      </c>
+      <c r="C175" s="15">
+        <v>0</v>
+      </c>
+      <c r="D175" s="15">
+        <v>1</v>
+      </c>
+      <c r="E175" s="15">
+        <v>0</v>
+      </c>
+      <c r="F175" s="15">
+        <v>1</v>
+      </c>
+      <c r="G175" s="17">
+        <v>0</v>
+      </c>
+      <c r="H175" s="17">
+        <v>0</v>
+      </c>
+      <c r="I175" s="17">
+        <v>0</v>
+      </c>
+      <c r="J175" s="17">
+        <v>0</v>
+      </c>
+      <c r="K175" s="15">
+        <v>0</v>
+      </c>
+      <c r="L175" s="15">
+        <v>1</v>
+      </c>
+      <c r="M175" s="15">
+        <v>0</v>
+      </c>
+      <c r="N175" s="15">
+        <v>1</v>
+      </c>
+      <c r="O175" s="15">
+        <v>0</v>
+      </c>
+      <c r="P175" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A176" s="1">
+        <v>12</v>
+      </c>
+      <c r="B176" s="15">
+        <v>0</v>
+      </c>
+      <c r="C176" s="15">
+        <v>1</v>
+      </c>
+      <c r="D176" s="17">
+        <v>0</v>
+      </c>
+      <c r="E176" s="17">
+        <v>0</v>
+      </c>
+      <c r="F176" s="17">
+        <v>0</v>
+      </c>
+      <c r="G176" s="17">
+        <v>0</v>
+      </c>
+      <c r="H176" s="15">
+        <v>1</v>
+      </c>
+      <c r="I176" s="15">
+        <v>0</v>
+      </c>
+      <c r="J176" s="15">
+        <v>0</v>
+      </c>
+      <c r="K176" s="15">
+        <v>0</v>
+      </c>
+      <c r="L176" s="15">
+        <v>0</v>
+      </c>
+      <c r="M176" s="15">
+        <v>0</v>
+      </c>
+      <c r="N176" s="15">
+        <v>0</v>
+      </c>
+      <c r="O176" s="15">
+        <v>1</v>
+      </c>
+      <c r="P176" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A177" s="1">
+        <v>13</v>
+      </c>
+      <c r="B177" s="17">
+        <v>0</v>
+      </c>
+      <c r="C177" s="17">
+        <v>0</v>
+      </c>
+      <c r="D177" s="17">
+        <v>0</v>
+      </c>
+      <c r="E177" s="15">
+        <v>1</v>
+      </c>
+      <c r="F177" s="15">
+        <v>0</v>
+      </c>
+      <c r="G177" s="15">
+        <v>0</v>
+      </c>
+      <c r="H177" s="15">
+        <v>1</v>
+      </c>
+      <c r="I177" s="15">
+        <v>0</v>
+      </c>
+      <c r="J177" s="15">
+        <v>1</v>
+      </c>
+      <c r="K177" s="15">
+        <v>1</v>
+      </c>
+      <c r="L177" s="15">
+        <v>1</v>
+      </c>
+      <c r="M177" s="15">
+        <v>1</v>
+      </c>
+      <c r="N177" s="15">
+        <v>0</v>
+      </c>
+      <c r="O177" s="15">
+        <v>1</v>
+      </c>
+      <c r="P177" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A178" s="1">
+        <v>14</v>
+      </c>
+      <c r="B178" s="12">
+        <v>0</v>
+      </c>
+      <c r="C178" s="15">
+        <v>1</v>
+      </c>
+      <c r="D178" s="15">
+        <v>0</v>
+      </c>
+      <c r="E178" s="15">
+        <v>0</v>
+      </c>
+      <c r="F178" s="15">
+        <v>0</v>
+      </c>
+      <c r="G178" s="15">
+        <v>0</v>
+      </c>
+      <c r="H178" s="15">
+        <v>1</v>
+      </c>
+      <c r="I178" s="15">
+        <v>0</v>
+      </c>
+      <c r="J178" s="15">
+        <v>0</v>
+      </c>
+      <c r="K178" s="15">
+        <v>0</v>
+      </c>
+      <c r="L178" s="15">
+        <v>0</v>
+      </c>
+      <c r="M178" s="15">
+        <v>0</v>
+      </c>
+      <c r="N178" s="15">
+        <v>0</v>
+      </c>
+      <c r="O178" s="15">
+        <v>1</v>
+      </c>
+      <c r="P178" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B179" s="5"/>
+      <c r="C179" s="5"/>
+      <c r="D179" s="5"/>
+      <c r="E179" s="5"/>
+      <c r="F179" s="5"/>
+      <c r="G179" s="5"/>
+      <c r="H179" s="5"/>
+      <c r="I179" s="5"/>
+      <c r="J179" s="5"/>
+      <c r="K179" s="5"/>
+      <c r="L179" s="5"/>
+      <c r="M179" s="5"/>
+    </row>
+    <row r="182" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A182" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B182" t="s">
+        <v>0</v>
+      </c>
+      <c r="C182" t="s">
+        <v>21</v>
+      </c>
+      <c r="D182" t="s">
+        <v>2</v>
+      </c>
+      <c r="E182" t="s">
+        <v>22</v>
+      </c>
+      <c r="F182" t="s">
+        <v>8</v>
+      </c>
+      <c r="G182">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="183" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A183" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B183" t="s">
+        <v>0</v>
+      </c>
+      <c r="C183" t="s">
+        <v>10</v>
+      </c>
+      <c r="D183" t="s">
+        <v>2</v>
+      </c>
+      <c r="E183" t="s">
+        <v>23</v>
+      </c>
+      <c r="F183" t="s">
+        <v>8</v>
+      </c>
+      <c r="G183">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F137355-BFCC-E841-9CED-17592919B9A2}">
+  <dimension ref="B3:N45"/>
+  <sheetViews>
+    <sheetView zoomScale="132" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30:C30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B5">
+        <v>64</v>
+      </c>
+      <c r="C5" s="18">
+        <v>0.69</v>
+      </c>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="19"/>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <v>100</v>
+      </c>
+      <c r="C6" s="18">
+        <v>0.7</v>
+      </c>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <v>120</v>
+      </c>
+      <c r="C7" s="18">
+        <v>0.75</v>
+      </c>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <v>225</v>
+      </c>
+      <c r="C8" s="18">
+        <v>0.75</v>
+      </c>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="19"/>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B9">
+        <v>255</v>
+      </c>
+      <c r="C9" s="18">
+        <v>0.8</v>
+      </c>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="19"/>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B10">
+        <v>288</v>
+      </c>
+      <c r="C10" s="18">
+        <v>1</v>
+      </c>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B11">
+        <v>324</v>
+      </c>
+      <c r="C11" s="18">
+        <v>1</v>
+      </c>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="19"/>
+      <c r="M11" s="19"/>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="19"/>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="19"/>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="19"/>
+      <c r="M14" s="19"/>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="19"/>
+      <c r="L15" s="19"/>
+      <c r="M15" s="19"/>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="19"/>
+      <c r="M16" s="19"/>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="19"/>
+      <c r="L17" s="19"/>
+      <c r="M17" s="19"/>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="19"/>
+      <c r="L18" s="19"/>
+      <c r="M18" s="19"/>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="19"/>
+      <c r="L19" s="19"/>
+      <c r="M19" s="19"/>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="19"/>
+      <c r="K20" s="19"/>
+      <c r="L20" s="19"/>
+      <c r="M20" s="19"/>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="19"/>
+      <c r="L21" s="19"/>
+      <c r="M21" s="19"/>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="G25" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="H25" s="21"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19"/>
+      <c r="K25" s="19"/>
+      <c r="L25" s="19"/>
+      <c r="M25" s="19"/>
+      <c r="N25" s="19"/>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" t="s">
+        <v>29</v>
+      </c>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="19"/>
+      <c r="L26" s="19"/>
+      <c r="M26" s="19"/>
+      <c r="N26" s="19"/>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B27">
+        <v>64</v>
+      </c>
+      <c r="C27">
+        <v>3.256E-5</v>
+      </c>
+      <c r="D27">
+        <v>6.5199999999999999E-5</v>
+      </c>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="19"/>
+      <c r="K27" s="19"/>
+      <c r="L27" s="19"/>
+      <c r="M27" s="19"/>
+      <c r="N27" s="19"/>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B28">
+        <v>100</v>
+      </c>
+      <c r="C28">
+        <f>C27*2</f>
+        <v>6.512E-5</v>
+      </c>
+      <c r="D28">
+        <f>D27*2</f>
+        <v>1.304E-4</v>
+      </c>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
+      <c r="K28" s="19"/>
+      <c r="L28" s="19"/>
+      <c r="M28" s="19"/>
+      <c r="N28" s="19"/>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B29">
+        <v>120</v>
+      </c>
+      <c r="C29">
+        <v>1.5699999999999999E-4</v>
+      </c>
+      <c r="D29">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="19"/>
+      <c r="K29" s="19"/>
+      <c r="L29" s="19"/>
+      <c r="M29" s="19"/>
+      <c r="N29" s="19"/>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B30">
+        <v>225</v>
+      </c>
+      <c r="C30">
+        <v>2.8699999999999998E-4</v>
+      </c>
+      <c r="D30">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="G30" s="19"/>
+      <c r="H30" s="19"/>
+      <c r="I30" s="19"/>
+      <c r="J30" s="19"/>
+      <c r="K30" s="19"/>
+      <c r="L30" s="19"/>
+      <c r="M30" s="19"/>
+      <c r="N30" s="19"/>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B31">
+        <v>255</v>
+      </c>
+      <c r="C31">
+        <v>3.5E-4</v>
+      </c>
+      <c r="D31">
+        <v>3.8999999999999999E-4</v>
+      </c>
+      <c r="G31" s="19"/>
+      <c r="H31" s="19"/>
+      <c r="I31" s="19"/>
+      <c r="J31" s="19"/>
+      <c r="K31" s="19"/>
+      <c r="L31" s="19"/>
+      <c r="M31" s="19"/>
+      <c r="N31" s="19"/>
+    </row>
+    <row r="32" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B32">
+        <v>288</v>
+      </c>
+      <c r="C32">
+        <v>4.1419999999999998E-4</v>
+      </c>
+      <c r="D32">
+        <v>4.5419999999999998E-4</v>
+      </c>
+      <c r="G32" s="19"/>
+      <c r="H32" s="19"/>
+      <c r="I32" s="19"/>
+      <c r="J32" s="19"/>
+      <c r="K32" s="19"/>
+      <c r="L32" s="19"/>
+      <c r="M32" s="19"/>
+      <c r="N32" s="19"/>
+    </row>
+    <row r="33" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B33">
+        <v>324</v>
+      </c>
+      <c r="C33">
+        <v>6.8749999999999996E-4</v>
+      </c>
+      <c r="D33">
+        <v>6.3849999999999996E-4</v>
+      </c>
+      <c r="G33" s="19"/>
+      <c r="H33" s="19"/>
+      <c r="I33" s="19"/>
+      <c r="J33" s="19"/>
+      <c r="K33" s="19"/>
+      <c r="L33" s="19"/>
+      <c r="M33" s="19"/>
+      <c r="N33" s="19"/>
+    </row>
+    <row r="34" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="G34" s="19"/>
+      <c r="H34" s="19"/>
+      <c r="I34" s="19"/>
+      <c r="J34" s="19"/>
+      <c r="K34" s="19"/>
+      <c r="L34" s="19"/>
+      <c r="M34" s="19"/>
+      <c r="N34" s="19"/>
+    </row>
+    <row r="35" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="G35" s="19"/>
+      <c r="H35" s="19"/>
+      <c r="I35" s="19"/>
+      <c r="J35" s="19"/>
+      <c r="K35" s="19"/>
+      <c r="L35" s="19"/>
+      <c r="M35" s="19"/>
+      <c r="N35" s="19"/>
+    </row>
+    <row r="36" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="G36" s="19"/>
+      <c r="H36" s="19"/>
+      <c r="I36" s="19"/>
+      <c r="J36" s="19"/>
+      <c r="K36" s="19"/>
+      <c r="L36" s="19"/>
+      <c r="M36" s="19"/>
+      <c r="N36" s="19"/>
+    </row>
+    <row r="37" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="G37" s="19"/>
+      <c r="H37" s="19"/>
+      <c r="I37" s="19"/>
+      <c r="J37" s="19"/>
+      <c r="K37" s="19"/>
+      <c r="L37" s="19"/>
+      <c r="M37" s="19"/>
+      <c r="N37" s="19"/>
+    </row>
+    <row r="38" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="G38" s="19"/>
+      <c r="H38" s="19"/>
+      <c r="I38" s="19"/>
+      <c r="J38" s="19"/>
+      <c r="K38" s="19"/>
+      <c r="L38" s="19"/>
+      <c r="M38" s="19"/>
+      <c r="N38" s="19"/>
+    </row>
+    <row r="39" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="G39" s="19"/>
+      <c r="H39" s="19"/>
+      <c r="I39" s="19"/>
+      <c r="J39" s="19"/>
+      <c r="K39" s="19"/>
+      <c r="L39" s="19"/>
+      <c r="M39" s="19"/>
+      <c r="N39" s="19"/>
+    </row>
+    <row r="40" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="G40" s="19"/>
+      <c r="H40" s="19"/>
+      <c r="I40" s="19"/>
+      <c r="J40" s="19"/>
+      <c r="K40" s="19"/>
+      <c r="L40" s="19"/>
+      <c r="M40" s="19"/>
+      <c r="N40" s="19"/>
+    </row>
+    <row r="41" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="G41" s="19"/>
+      <c r="H41" s="19"/>
+      <c r="I41" s="19"/>
+      <c r="J41" s="19"/>
+      <c r="K41" s="19"/>
+      <c r="L41" s="19"/>
+      <c r="M41" s="19"/>
+    </row>
+    <row r="42" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="G42" s="19"/>
+      <c r="H42" s="19"/>
+      <c r="I42" s="19"/>
+      <c r="J42" s="19"/>
+      <c r="K42" s="19"/>
+      <c r="L42" s="19"/>
+      <c r="M42" s="19"/>
+      <c r="N42" s="19"/>
+    </row>
+    <row r="43" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="G43" s="19"/>
+      <c r="H43" s="19"/>
+      <c r="I43" s="19"/>
+      <c r="J43" s="19"/>
+      <c r="K43" s="19"/>
+      <c r="L43" s="19"/>
+      <c r="M43" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="N43" s="19"/>
+    </row>
+    <row r="44" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="G44" s="19"/>
+      <c r="H44" s="19"/>
+      <c r="I44" s="19"/>
+      <c r="J44" s="19"/>
+      <c r="K44" s="19"/>
+      <c r="L44" s="19"/>
+      <c r="M44" s="19"/>
+      <c r="N44" s="19"/>
+    </row>
+    <row r="45" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="G45" s="19"/>
+      <c r="H45" s="19"/>
+      <c r="I45" s="19"/>
+      <c r="J45" s="19"/>
+      <c r="K45" s="19"/>
+      <c r="L45" s="19"/>
+      <c r="M45" s="19"/>
+      <c r="N45" s="19"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="G25:H25"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>